<commit_message>
Commit generate password on number of characters
</commit_message>
<xml_diff>
--- a/Endchoice.xlsx
+++ b/Endchoice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trang\TrangTheDev\BootCamp\Homework_week3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB611CD-DE04-4546-87C6-1FD1ED732D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C6E6617-0CE6-4131-9579-D03F58577195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" xr2:uid="{762AC876-ED48-4BF3-83F8-1533523A5189}"/>
+    <workbookView xWindow="7815" yWindow="4777" windowWidth="3870" windowHeight="3826" xr2:uid="{762AC876-ED48-4BF3-83F8-1533523A5189}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -683,7 +683,7 @@
   <dimension ref="E8:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>